<commit_message>
Final version for Koli Calling 2025
</commit_message>
<xml_diff>
--- a/other_contexts.xlsx
+++ b/other_contexts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Which paper</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Context</t>
   </si>
   <si>
+    <t>2018_2c</t>
+  </si>
+  <si>
     <t>2019_3294016.3294021</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t>2025_3702212.3702225</t>
   </si>
   <si>
+    <t>2c. The enemies within - inhibitors to learning</t>
+  </si>
+  <si>
     <t>Data Protection and Privacy Regulations as an  Inter-Active-Constructive Practice</t>
   </si>
   <si>
@@ -154,6 +160,9 @@
     <t>Integrating Socially Responsible Computing Competencies in Computer Science and Software Engineering Education</t>
   </si>
   <si>
+    <t>policy setting</t>
+  </si>
+  <si>
     <t>cybersecurity</t>
   </si>
   <si>
@@ -173,6 +182,9 @@
   </si>
   <si>
     <t>cloud computing</t>
+  </si>
+  <si>
+    <t>Cloud computing</t>
   </si>
   <si>
     <t>training for early year academics in teaching computing</t>
@@ -572,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -591,161 +603,161 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -754,12 +766,12 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -768,133 +780,161 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>203</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>205</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>